<commit_message>
è tutto vero signori
</commit_message>
<xml_diff>
--- a/Working_data/amoco_HN.xlsx
+++ b/Working_data/amoco_HN.xlsx
@@ -1117,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1168,32 +1168,9 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>1.5</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1</v>
-      </c>
-      <c r="C3" t="str">
-        <v>1</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>1</v>
-      </c>
-      <c r="F3" t="str">
-        <v>0.8</v>
-      </c>
-      <c r="G3" t="str">
-        <v>0.8</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New discretization. Control System approach and validation
</commit_message>
<xml_diff>
--- a/Working_data/amoco_HN.xlsx
+++ b/Working_data/amoco_HN.xlsx
@@ -1117,7 +1117,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1162,15 +1162,38 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
+        <v>0.9956</v>
+      </c>
+      <c r="G2" t="str">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
         <v>1.2</v>
       </c>
-      <c r="G2" t="str">
-        <v>1.2</v>
+      <c r="G3" t="str">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>